<commit_message>
add main and search page
</commit_message>
<xml_diff>
--- a/src/main/resources/Test_Data.xlsx
+++ b/src/main/resources/Test_Data.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUY.NX183556\java\eclipse\workspace\DoAn_2023\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18360" windowHeight="3360"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Sign_In" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>STT</t>
   </si>
@@ -495,7 +499,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add condition Pass for SignIn
</commit_message>
<xml_diff>
--- a/src/main/resources/Test_Data.xlsx
+++ b/src/main/resources/Test_Data.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUY.NX183556\java\eclipse\workspace\DoAn_2023\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18360" windowHeight="3360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18360" windowHeight="5550"/>
   </bookViews>
   <sheets>
     <sheet name="Sign_In" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>STT</t>
   </si>
@@ -41,33 +41,9 @@
     <t>Results</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>SignIn_TC1</t>
-  </si>
-  <si>
-    <t>Mozilla</t>
-  </si>
-  <si>
-    <t>SignIn_TC2</t>
-  </si>
-  <si>
-    <t>SignIn_TC3</t>
-  </si>
-  <si>
-    <t>SignIn_TC4</t>
-  </si>
-  <si>
     <t>Đăng nhập khi để trống pass</t>
   </si>
   <si>
-    <t>SignIn_TC5</t>
-  </si>
-  <si>
-    <t>SignIn_TC6</t>
-  </si>
-  <si>
     <t>Đăng nhập đúng email và password</t>
   </si>
   <si>
@@ -95,7 +71,34 @@
     <t>Huy1631734911234@</t>
   </si>
   <si>
-    <t>Fail</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Expectation key</t>
+  </si>
+  <si>
+    <t>Expectation result</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> //span[text()='Install App']</t>
+  </si>
+  <si>
+    <t>//span[text()='Incorrect username or password.']</t>
   </si>
   <si>
     <t>Pass</t>
@@ -105,7 +108,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,7 +186,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -214,6 +216,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -496,23 +507,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="35.42578125" style="12" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="38.7109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,110 +541,129 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="F3" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="13"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="4" t="s">
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="D7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G7" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
add search and filter
</commit_message>
<xml_diff>
--- a/src/main/resources/Test_Data.xlsx
+++ b/src/main/resources/Test_Data.xlsx
@@ -3,20 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUY.NX183556\java\eclipse\workspace\DoAn_2023\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18360" windowHeight="5550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18360" windowHeight="5550" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sign_In" sheetId="1" r:id="rId1"/>
+    <sheet name="Search" sheetId="2" r:id="rId2"/>
+    <sheet name="Add_Playlist" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>STT</t>
   </si>
@@ -102,12 +104,88 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>SearchText</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhập đầy đủ tên một bài hát </t>
+  </si>
+  <si>
+    <t>Nơi này có anh</t>
+  </si>
+  <si>
+    <t>Hiển thị bài hát nơi này có anh trên trang web</t>
+  </si>
+  <si>
+    <t>//div[@class='sm7ZnbOO1Zfg9cupYgPN']/a[@title='Nơi Này Có Anh']</t>
+  </si>
+  <si>
+    <t>Tìm kiếm tên đầy đủ của ca sĩ hoặc nhạc sĩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sơn Tùng </t>
+  </si>
+  <si>
+    <t>Hiển thị tên nghệ sĩ Sơn Tùng trên trang</t>
+  </si>
+  <si>
+    <t>//div[@class='sm7ZnbOO1Zfg9cupYgPN']/a[@title='Sơn Tùng M-TP']</t>
+  </si>
+  <si>
+    <t>Tìm kiếm thể loại nhạc</t>
+  </si>
+  <si>
+    <t>hiphop</t>
+  </si>
+  <si>
+    <t>//div[@class='sm7ZnbOO1Zfg9cupYgPN']/a[@title='Hip-Hop']</t>
+  </si>
+  <si>
+    <t>Tìm kiếm mờ: Tên gần đúng một bài hát</t>
+  </si>
+  <si>
+    <t>Nơi này</t>
+  </si>
+  <si>
+    <t>Tìm kiếm mờ: Tên gần đúng 1 nghệ sĩ</t>
+  </si>
+  <si>
+    <t>Sơn</t>
+  </si>
+  <si>
+    <t>Hiển thị tên thể loại hiphop trên trang</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Nhập dữ liệu vào ô search + filter theo Songs</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>//span[text()='Songs']/parent::button</t>
+  </si>
+  <si>
+    <t>//a[text()='Adele']</t>
+  </si>
+  <si>
+    <t>Hiển thị bài hát Hello - Adele muốn tìm</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -186,7 +264,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -224,6 +302,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -509,19 +602,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="35.42578125" style="12" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="38.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="12" width="35.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="12" width="38.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -678,4 +771,194 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="17" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="17" width="35.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="17" width="39.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="17" width="39.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="17" width="33.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="17" width="28.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="17" width="31.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update test for add play list
</commit_message>
<xml_diff>
--- a/src/main/resources/Test_Data.xlsx
+++ b/src/main/resources/Test_Data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>STT</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>Hiển thị bài hát Hello - Adele muốn tìm</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -775,18 +772,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="17" width="10.42578125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="17" width="35.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="17" width="39.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="17" width="39.140625" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" style="17" width="39.140625" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="17" width="33.5703125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="17" width="28.85546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="17" width="31.85546875" collapsed="true"/>
@@ -836,6 +832,27 @@
       </c>
       <c r="G2" s="16" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +865,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G5"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>